<commit_message>
Looking at first alternate solution
</commit_message>
<xml_diff>
--- a/CH-84 Normal Distribution.xlsx
+++ b/CH-84 Normal Distribution.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA40B9A0-310A-4E60-A7B9-F35DB85A831D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F2D102-8C3C-4EA8-B64D-1E2D6B707E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$N$3:$O$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$N$3:$O$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$N$3:$O$4</definedName>
   </definedNames>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Z</t>
   </si>
@@ -90,10 +92,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -426,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -528,10 +531,11 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1531,6 +1535,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="858" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0181A599-7D8F-4FE3-93BF-A24973C764A9}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
@@ -1550,19 +1581,19 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
       <c r="N1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2053,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50AB575-EC42-4E43-8A2B-17C63E38866C}">
   <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -2077,19 +2108,19 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
       <c r="N1" s="25" t="s">
         <v>1</v>
       </c>
@@ -2587,7 +2618,7 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B18" s="36" cm="1">
+      <c r="B18" s="35" cm="1">
         <f t="array" ref="B18:B127">_xlfn.TOCOL(B3:B13+C2:L2)</f>
         <v>0</v>
       </c>
@@ -3556,6 +3587,564 @@
       </c>
       <c r="C127" s="2">
         <v>0.36209999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7606F015-793F-4926-B0BC-9791639C7209}">
+  <dimension ref="A1:O23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="5.69921875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="5.8984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.296875" style="2" customWidth="1"/>
+    <col min="5" max="12" width="5.8984375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9" style="2"/>
+    <col min="14" max="15" width="14.8984375" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2"/>
+      <c r="B1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="N1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="H2" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="I2" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="J2" s="16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K2" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="L2" s="17">
+        <v>0.09</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E3" s="9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="I3" s="9">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="J3" s="9">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="K3" s="9">
+        <v>3.1899999999999998E-2</v>
+      </c>
+      <c r="L3" s="10">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="N3" s="26">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="O3" s="27">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B4" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="E4" s="18">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5.1700000000000003E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5.57E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5.96E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="K4" s="4">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="L4" s="5">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="N4" s="28">
+        <v>0.17</v>
+      </c>
+      <c r="O4" s="27">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B5" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="11">
+        <v>7.9299999999999995E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>8.7099999999999997E-2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>9.8699999999999996E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.1026</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.10639999999999999</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.1103</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.11409999999999999</v>
+      </c>
+      <c r="N5" s="29">
+        <v>0.2823</v>
+      </c>
+      <c r="O5" s="27">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B6" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.1179</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.1217</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.1255</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.1293</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.1331</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.1368</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.1406</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.14430000000000001</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.1517</v>
+      </c>
+      <c r="N6" s="30">
+        <v>0.33150000000000002</v>
+      </c>
+      <c r="O6" s="27">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B7" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.15540000000000001</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.15909999999999999</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.1628</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.16639999999999999</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0.17</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.1736</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.1772</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.18079999999999999</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0.18440000000000001</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.18790000000000001</v>
+      </c>
+      <c r="N7" s="31">
+        <v>0.32379999999999998</v>
+      </c>
+      <c r="O7" s="27">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B8" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.1915</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.19850000000000001</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.2019</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.2054</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.20880000000000001</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.21229999999999999</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.2157</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.219</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.22239999999999999</v>
+      </c>
+      <c r="N8" s="32">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="O8" s="27">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B9" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.22570000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.2291</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.2324</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.23569999999999999</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.2389</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.2422</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.24540000000000001</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.24859999999999999</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.25490000000000002</v>
+      </c>
+      <c r="N9" s="33">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="O9" s="27">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B10" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.2611</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.26419999999999999</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.26729999999999998</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.27039999999999997</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.27939999999999998</v>
+      </c>
+      <c r="K10" s="20">
+        <v>0.2823</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.28520000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B11" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.29389999999999999</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.29949999999999999</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.30780000000000002</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.31059999999999999</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.31330000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B12" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0.31590000000000001</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.31859999999999999</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.32119999999999999</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0.32379999999999998</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.32640000000000002</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.32890000000000003</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.33150000000000002</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="K12" s="23">
+        <v>0.33650000000000002</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.33889999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.34129999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.34610000000000002</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.34849999999999998</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.3508</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.35310000000000002</v>
+      </c>
+      <c r="I13" s="24">
+        <v>0.35539999999999999</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0.35770000000000002</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.3599</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0.36209999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O17" s="37" cm="1">
+        <f t="array" ref="O17:O23">_xlfn.LET(
+_xlpm.a, _xlfn.TEXTSPLIT(_xlfn.TEXTJOIN(",",TRUE,C2:L2&amp;"-"&amp;B3:B13&amp;"-"&amp;C3:L13),"-",",")*1,
+_xlpm.b, _xlfn.BYROW(N3:N9, _xlfn.LAMBDA(_xlpm.x, SUM(_xlfn.XLOOKUP(_xlpm.x,_xlfn.TAKE(_xlpm.a,,-1),_xlfn.TAKE(_xlpm.a,,2),,-1)))),
+_xlpm.b
+)</f>
+        <v>0.12000000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O18" s="37">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="19" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O19" s="37">
+        <v>0.77999999999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O20" s="37">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="21" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O21" s="37">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="22" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O22" s="37">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="23" spans="15:15" x14ac:dyDescent="0.4">
+      <c r="O23" s="37">
+        <v>1.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>